<commit_message>
Update imported xlsx file
</commit_message>
<xml_diff>
--- a/imported.xlsx
+++ b/imported.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>ชื่อสินค้า</t>
   </si>
@@ -22,10 +22,16 @@
     <t>ต้องการมากๆ</t>
   </si>
   <si>
-    <t>หมูสับ</t>
+    <t>ซีพียู</t>
   </si>
   <si>
-    <t>ไข่ดาว</t>
+    <t>เมนบอร์ด</t>
+  </si>
+  <si>
+    <t>แรม</t>
+  </si>
+  <si>
+    <t>โคมไฟตั้งพื้น</t>
   </si>
 </sst>
 </file>
@@ -35,7 +41,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -53,7 +59,12 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="10"/>
+      <sz val="16"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -78,7 +89,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -105,6 +116,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -114,6 +147,24 @@
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -131,13 +182,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -147,16 +265,49 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -180,6 +331,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1241,17 +1393,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.0859" style="1" customWidth="1"/>
+    <col min="2" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21.85" customHeight="1">
+    <row r="1" ht="34.95" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
@@ -1261,28 +1414,109 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
-    <row r="2" ht="21.85" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" ht="36.25" customHeight="1">
+      <c r="A2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
-        <v>20</v>
+      <c r="B2" s="6">
+        <v>7000</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" ht="36.75" customHeight="1">
+      <c r="A3" t="s" s="9">
+        <v>4</v>
+      </c>
+      <c r="B3" s="10">
+        <v>6000</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" ht="35.25" customHeight="1">
+      <c r="A4" t="s" s="9">
+        <v>5</v>
+      </c>
+      <c r="B4" s="10">
+        <v>3500</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" ht="40.6" customHeight="1">
+      <c r="A5" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2500</v>
+      </c>
+      <c r="C5" s="10">
         <v>1</v>
       </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
     </row>
-    <row r="3" ht="21.65" customHeight="1">
-      <c r="A3" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6">
-        <v>10</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="14"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" ht="14.7" customHeight="1">
+      <c r="A11" s="14"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" ht="14.7" customHeight="1">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>